<commit_message>
added information pertaining to Mac OS, Safari and Selenium Actions incompatibility
</commit_message>
<xml_diff>
--- a/Broswer-OS Matrix Selenium TestNG parameters.xlsx
+++ b/Broswer-OS Matrix Selenium TestNG parameters.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="16380" windowHeight="11055"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="15045" windowHeight="6630"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:J8"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Browser / OS</t>
   </si>
@@ -123,13 +124,16 @@
   </si>
   <si>
     <t>IE 10 is Win8, and IE 11 is win 8.1</t>
+  </si>
+  <si>
+    <t>An issue exists with Safari 7 and 8 and Selennium Actions. The issue can be tracked here.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,8 +156,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -184,8 +196,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -260,11 +278,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF6D6D6D"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -295,8 +323,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -596,10 +631,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,9 +643,10 @@
     <col min="2" max="2" width="17.7109375" customWidth="1"/>
     <col min="3" max="3" width="17.140625" customWidth="1"/>
     <col min="4" max="4" width="26.28515625" customWidth="1"/>
+    <col min="5" max="5" width="45.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -624,7 +660,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -636,7 +672,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -648,7 +684,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -662,7 +698,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -676,7 +712,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -684,42 +720,46 @@
       <c r="C6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="12" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E6" s="13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="12" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="13"/>
+    </row>
+    <row r="10" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="8"/>
       <c r="C10" s="10" t="s">
         <v>19</v>
       </c>
       <c r="D10" s="10"/>
     </row>
-    <row r="11" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="9"/>
       <c r="C11" s="10" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="10"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" s="11" t="s">
         <v>25</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="11"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="11" t="s">
         <v>26</v>
       </c>
@@ -727,14 +767,18 @@
       <c r="D15" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="B14:D14"/>
+    <mergeCell ref="E6:E7"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="E6:E7" r:id="rId1" display="An issue exists with Safari 7 and 8 and Selennium Actions. The issue can be tracked here."/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>